<commit_message>
UI ~90% presentable, Just need to connect UI to TB UI
</commit_message>
<xml_diff>
--- a/Track_Model/Blue Line.xlsx
+++ b/Track_Model/Blue Line.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DRich\PycharmProjects\ece1140-tovarish\Track_Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6564752A-1BB3-4582-9D41-F11F63EC7136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5C5379-727C-4EF9-ABA0-382265E21FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="11010" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -541,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TestBench reading to main window
</commit_message>
<xml_diff>
--- a/Track_Model/Blue Line.xlsx
+++ b/Track_Model/Blue Line.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DRich\PycharmProjects\ece1140-tovarish\Track_Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5C5379-727C-4EF9-ABA0-382265E21FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212FEC58-0FB7-477B-A757-90FDE62093EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Line</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Broken Rail Failure</t>
+  </si>
+  <si>
+    <t>Embarking</t>
+  </si>
+  <si>
+    <t>Ticket Sales</t>
   </si>
 </sst>
 </file>
@@ -539,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,10 +565,12 @@
     <col min="11" max="11" width="8" style="7" customWidth="1"/>
     <col min="12" max="12" width="15.85546875" style="7" customWidth="1"/>
     <col min="13" max="13" width="15" style="7" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="7"/>
+    <col min="14" max="16" width="9.140625" style="7"/>
+    <col min="17" max="18" width="11.5703125" style="7" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="63" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -611,8 +619,14 @@
       <c r="P1" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -653,7 +667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f>A2</f>
         <v>Blue</v>
@@ -695,7 +709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A16" si="0">A3</f>
         <v>Blue</v>
@@ -741,7 +755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Blue</v>
@@ -783,7 +797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Blue</v>
@@ -829,7 +843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Blue</v>
@@ -875,7 +889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Blue</v>
@@ -917,7 +931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Blue</v>
@@ -959,7 +973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Blue</v>
@@ -1008,7 +1022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Blue</v>
@@ -1056,8 +1070,14 @@
       <c r="P11" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q11" s="7">
+        <v>0</v>
+      </c>
+      <c r="R11" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Blue</v>
@@ -1103,7 +1123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Blue</v>
@@ -1145,7 +1165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Blue</v>
@@ -1187,7 +1207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Blue</v>
@@ -1236,7 +1256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Blue</v>
@@ -1282,6 +1302,12 @@
         <v>0</v>
       </c>
       <c r="P16" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="7">
+        <v>0</v>
+      </c>
+      <c r="R16" s="7">
         <v>0</v>
       </c>
     </row>

</xml_diff>